<commit_message>
adding cases in excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/SignUp_data.xlsx
+++ b/src/test/resources/SignUp_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
   <si>
     <t>first_name</t>
   </si>
@@ -50,13 +50,91 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Learning AutoTest</t>
+  </si>
+  <si>
+    <t>client_test@</t>
+  </si>
+  <si>
+    <t>email address is not a valid email address</t>
+  </si>
+  <si>
+    <t>@example.com</t>
+  </si>
+  <si>
+    <t>email address is not a valid email address,email address is required</t>
+  </si>
+  <si>
+    <t>client.com</t>
+  </si>
+  <si>
+    <t>mike@example.com</t>
+  </si>
+  <si>
+    <t>email address is already taken</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>password is required</t>
+  </si>
+  <si>
+    <t>123457</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>t@e.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> client_test@example.com </t>
+  </si>
+  <si>
+    <t>Tester!</t>
+  </si>
+  <si>
+    <t>Demo@</t>
+  </si>
+  <si>
+    <t>Learning# AutoTest$</t>
+  </si>
+  <si>
+    <t>client_test_1@example.com</t>
+  </si>
+  <si>
+    <t>%123456</t>
+  </si>
+  <si>
+    <t>client_test_2@example.com</t>
+  </si>
+  <si>
+    <t>confirm password does not match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,12 +149,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF17C6A3"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -132,16 +204,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,13 +595,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -550,17 +631,103 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +759,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -617,21 +784,273 @@
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4" display="client_test@"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+    <hyperlink ref="D14" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>